<commit_message>
ตรวจ Class Diagram Controller และ Model
</commit_message>
<xml_diff>
--- a/ตรวจงาน/รายการตรวจสอบแผนภาพ.xlsx
+++ b/ตรวจงาน/รายการตรวจสอบแผนภาพ.xlsx
@@ -1,31 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nice-\Desktop\Porn\TEAM4\team4\ตรวจงาน\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\team4\ตรวจงาน\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{852934E5-DE33-4A29-AB80-4E659C78761E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52149E89-A034-4E4D-92ED-AFDF6884F31B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5940" yWindow="1080" windowWidth="21060" windowHeight="14175" xr2:uid="{C108298C-C5B1-4B19-85F2-2856099ECD84}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C108298C-C5B1-4B19-85F2-2856099ECD84}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="47">
   <si>
     <t>คำผิด</t>
   </si>
@@ -160,17 +165,23 @@
   </si>
   <si>
     <t>V1.1.2</t>
+  </si>
+  <si>
+    <t>Class Diagram Controller</t>
+  </si>
+  <si>
+    <t>Class Diagram Model</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -190,13 +201,13 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,6 +229,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -275,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -314,6 +331,24 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -323,27 +358,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -359,7 +379,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ธีมของ Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -658,103 +678,103 @@
   <dimension ref="B2:W168"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+      <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="30" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="1"/>
-    <col min="2" max="2" width="36.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="1"/>
-    <col min="4" max="4" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="8.75" style="1"/>
+    <col min="2" max="2" width="36.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.75" style="1"/>
+    <col min="4" max="4" width="10.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:23" ht="50.45" customHeight="1">
-      <c r="B2" s="16" t="s">
+    <row r="2" spans="2:23" ht="50.45" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="M2" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="N2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="17" t="s">
+      <c r="O2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="21" t="s">
+      <c r="P2" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="Q2" s="17" t="s">
+      <c r="Q2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="R2" s="17" t="s">
+      <c r="R2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-    </row>
-    <row r="3" spans="2:23" ht="51.75" customHeight="1">
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="14"/>
+      <c r="W2" s="14"/>
+    </row>
+    <row r="3" spans="2:23" ht="51.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
       <c r="E3" s="19"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="20"/>
-      <c r="T3" s="20"/>
-      <c r="U3" s="20"/>
-      <c r="V3" s="20"/>
-      <c r="W3" s="20"/>
-    </row>
-    <row r="4" spans="2:23" ht="30" customHeight="1">
-      <c r="B4" s="14" t="s">
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="14"/>
+      <c r="W3" s="14"/>
+    </row>
+    <row r="4" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" s="20" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -794,8 +814,8 @@
       <c r="V4" s="4"/>
       <c r="W4" s="4"/>
     </row>
-    <row r="5" spans="2:23" ht="30" customHeight="1">
-      <c r="B5" s="15"/>
+    <row r="5" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="21"/>
       <c r="C5" s="2" t="s">
         <v>20</v>
       </c>
@@ -829,7 +849,7 @@
       <c r="V5" s="4"/>
       <c r="W5" s="4"/>
     </row>
-    <row r="6" spans="2:23" ht="30" customHeight="1">
+    <row r="6" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="11" t="s">
         <v>22</v>
       </c>
@@ -867,7 +887,7 @@
       <c r="V6" s="4"/>
       <c r="W6" s="4"/>
     </row>
-    <row r="7" spans="2:23" ht="30" customHeight="1">
+    <row r="7" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="11" t="s">
         <v>25</v>
       </c>
@@ -905,7 +925,7 @@
       <c r="V7" s="4"/>
       <c r="W7" s="4"/>
     </row>
-    <row r="8" spans="2:23" ht="30" customHeight="1">
+    <row r="8" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="11" t="s">
         <v>26</v>
       </c>
@@ -943,7 +963,7 @@
       <c r="V8" s="4"/>
       <c r="W8" s="4"/>
     </row>
-    <row r="9" spans="2:23" ht="30" customHeight="1">
+    <row r="9" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="11" t="s">
         <v>28</v>
       </c>
@@ -981,7 +1001,7 @@
       <c r="V9" s="4"/>
       <c r="W9" s="4"/>
     </row>
-    <row r="10" spans="2:23" ht="30" customHeight="1">
+    <row r="10" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="11" t="s">
         <v>29</v>
       </c>
@@ -1019,7 +1039,7 @@
       <c r="V10" s="4"/>
       <c r="W10" s="4"/>
     </row>
-    <row r="11" spans="2:23" ht="30" customHeight="1">
+    <row r="11" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="11" t="s">
         <v>30</v>
       </c>
@@ -1057,7 +1077,7 @@
       <c r="V11" s="4"/>
       <c r="W11" s="4"/>
     </row>
-    <row r="12" spans="2:23" ht="30" customHeight="1">
+    <row r="12" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="12" t="s">
         <v>31</v>
       </c>
@@ -1098,7 +1118,7 @@
       <c r="V12" s="4"/>
       <c r="W12" s="4"/>
     </row>
-    <row r="13" spans="2:23" ht="31.9" customHeight="1">
+    <row r="13" spans="2:23" ht="31.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="13" t="s">
         <v>38</v>
       </c>
@@ -1139,7 +1159,7 @@
       <c r="V13" s="4"/>
       <c r="W13" s="4"/>
     </row>
-    <row r="14" spans="2:23" ht="30" customHeight="1">
+    <row r="14" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="13" t="s">
         <v>35</v>
       </c>
@@ -1176,7 +1196,7 @@
       <c r="V14" s="4"/>
       <c r="W14" s="4"/>
     </row>
-    <row r="15" spans="2:23" ht="30" customHeight="1">
+    <row r="15" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="13" t="s">
         <v>36</v>
       </c>
@@ -1219,7 +1239,7 @@
       <c r="V15" s="4"/>
       <c r="W15" s="4"/>
     </row>
-    <row r="16" spans="2:23" ht="30" customHeight="1">
+    <row r="16" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="13" t="s">
         <v>37</v>
       </c>
@@ -1262,7 +1282,7 @@
       <c r="V16" s="4"/>
       <c r="W16" s="4"/>
     </row>
-    <row r="17" spans="2:23" ht="30" customHeight="1">
+    <row r="17" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="13" t="s">
         <v>39</v>
       </c>
@@ -1301,7 +1321,7 @@
       <c r="V17" s="4"/>
       <c r="W17" s="4"/>
     </row>
-    <row r="18" spans="2:23" ht="30" customHeight="1">
+    <row r="18" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="11" t="s">
         <v>25</v>
       </c>
@@ -1337,7 +1357,7 @@
       <c r="V18" s="4"/>
       <c r="W18" s="4"/>
     </row>
-    <row r="19" spans="2:23" ht="30" customHeight="1">
+    <row r="19" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="11" t="s">
         <v>43</v>
       </c>
@@ -1373,7 +1393,7 @@
       <c r="V19" s="4"/>
       <c r="W19" s="4"/>
     </row>
-    <row r="20" spans="2:23" ht="30" customHeight="1">
+    <row r="20" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="11" t="s">
         <v>30</v>
       </c>
@@ -1409,55 +1429,93 @@
       <c r="V20" s="4"/>
       <c r="W20" s="4"/>
     </row>
-    <row r="21" spans="2:23" ht="30" customHeight="1">
-      <c r="B21" s="5"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+    <row r="21" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B21" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="3">
+        <v>242724</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1</v>
+      </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
+      <c r="J21" s="2">
+        <v>50</v>
+      </c>
       <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
+      <c r="L21" s="2">
+        <v>31</v>
+      </c>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
-      <c r="Q21" s="2"/>
-      <c r="R21" s="2"/>
+      <c r="Q21" s="2">
+        <v>3</v>
+      </c>
+      <c r="R21" s="2">
+        <f>SUM(F21:Q21)</f>
+        <v>85</v>
+      </c>
       <c r="S21" s="4"/>
       <c r="T21" s="4"/>
       <c r="U21" s="4"/>
       <c r="V21" s="4"/>
       <c r="W21" s="4"/>
     </row>
-    <row r="22" spans="2:23" ht="30" customHeight="1">
-      <c r="B22" s="5"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+    <row r="22" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="3">
+        <v>242724</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
+      <c r="J22" s="2">
+        <v>15</v>
+      </c>
+      <c r="K22" s="2">
+        <v>6</v>
+      </c>
+      <c r="L22" s="2">
+        <v>2</v>
+      </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
-      <c r="Q22" s="2"/>
-      <c r="R22" s="2"/>
+      <c r="Q22" s="2">
+        <v>2</v>
+      </c>
+      <c r="R22" s="2">
+        <f>SUM(F22:Q22)</f>
+        <v>25</v>
+      </c>
       <c r="S22" s="4"/>
       <c r="T22" s="4"/>
       <c r="U22" s="4"/>
       <c r="V22" s="4"/>
       <c r="W22" s="4"/>
     </row>
-    <row r="23" spans="2:23" ht="30" customHeight="1">
+    <row r="23" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" s="5"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -1481,7 +1539,7 @@
       <c r="V23" s="4"/>
       <c r="W23" s="4"/>
     </row>
-    <row r="24" spans="2:23" ht="30" customHeight="1">
+    <row r="24" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" s="5"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -1505,7 +1563,7 @@
       <c r="V24" s="4"/>
       <c r="W24" s="4"/>
     </row>
-    <row r="25" spans="2:23" ht="30" customHeight="1">
+    <row r="25" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" s="5"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1529,7 +1587,7 @@
       <c r="V25" s="4"/>
       <c r="W25" s="4"/>
     </row>
-    <row r="26" spans="2:23" ht="30" customHeight="1">
+    <row r="26" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B26" s="5"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1553,7 +1611,7 @@
       <c r="V26" s="4"/>
       <c r="W26" s="4"/>
     </row>
-    <row r="27" spans="2:23" ht="30" customHeight="1">
+    <row r="27" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B27" s="5"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1577,7 +1635,7 @@
       <c r="V27" s="4"/>
       <c r="W27" s="4"/>
     </row>
-    <row r="28" spans="2:23" ht="30" customHeight="1">
+    <row r="28" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B28" s="5"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -1601,7 +1659,7 @@
       <c r="V28" s="4"/>
       <c r="W28" s="4"/>
     </row>
-    <row r="29" spans="2:23" ht="30" customHeight="1">
+    <row r="29" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" s="5"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1625,7 +1683,7 @@
       <c r="V29" s="4"/>
       <c r="W29" s="4"/>
     </row>
-    <row r="30" spans="2:23" ht="30" customHeight="1">
+    <row r="30" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B30" s="5"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -1649,7 +1707,7 @@
       <c r="V30" s="4"/>
       <c r="W30" s="4"/>
     </row>
-    <row r="31" spans="2:23" ht="30" customHeight="1">
+    <row r="31" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B31" s="5"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -1673,7 +1731,7 @@
       <c r="V31" s="4"/>
       <c r="W31" s="4"/>
     </row>
-    <row r="32" spans="2:23" ht="30" customHeight="1">
+    <row r="32" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B32" s="5"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -1697,7 +1755,7 @@
       <c r="V32" s="4"/>
       <c r="W32" s="4"/>
     </row>
-    <row r="33" spans="2:23" ht="30" customHeight="1">
+    <row r="33" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B33" s="5"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -1721,7 +1779,7 @@
       <c r="V33" s="4"/>
       <c r="W33" s="4"/>
     </row>
-    <row r="34" spans="2:23" ht="30" customHeight="1">
+    <row r="34" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B34" s="5"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -1745,7 +1803,7 @@
       <c r="V34" s="4"/>
       <c r="W34" s="4"/>
     </row>
-    <row r="35" spans="2:23" ht="30" customHeight="1">
+    <row r="35" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B35" s="5"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -1769,7 +1827,7 @@
       <c r="V35" s="4"/>
       <c r="W35" s="4"/>
     </row>
-    <row r="36" spans="2:23" ht="30" customHeight="1">
+    <row r="36" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B36" s="5"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -1793,7 +1851,7 @@
       <c r="V36" s="4"/>
       <c r="W36" s="4"/>
     </row>
-    <row r="37" spans="2:23" ht="30" customHeight="1">
+    <row r="37" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B37" s="5"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -1817,7 +1875,7 @@
       <c r="V37" s="4"/>
       <c r="W37" s="4"/>
     </row>
-    <row r="38" spans="2:23" ht="30" customHeight="1">
+    <row r="38" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B38" s="5"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -1841,7 +1899,7 @@
       <c r="V38" s="4"/>
       <c r="W38" s="4"/>
     </row>
-    <row r="39" spans="2:23" ht="30" customHeight="1">
+    <row r="39" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B39" s="5"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -1865,7 +1923,7 @@
       <c r="V39" s="4"/>
       <c r="W39" s="4"/>
     </row>
-    <row r="40" spans="2:23" ht="30" customHeight="1">
+    <row r="40" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B40" s="5"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -1889,7 +1947,7 @@
       <c r="V40" s="4"/>
       <c r="W40" s="4"/>
     </row>
-    <row r="41" spans="2:23" ht="30" customHeight="1">
+    <row r="41" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B41" s="5"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -1913,7 +1971,7 @@
       <c r="V41" s="4"/>
       <c r="W41" s="4"/>
     </row>
-    <row r="42" spans="2:23" ht="30" customHeight="1">
+    <row r="42" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B42" s="5"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -1937,7 +1995,7 @@
       <c r="V42" s="4"/>
       <c r="W42" s="4"/>
     </row>
-    <row r="43" spans="2:23" ht="30" customHeight="1">
+    <row r="43" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B43" s="5"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -1961,7 +2019,7 @@
       <c r="V43" s="4"/>
       <c r="W43" s="4"/>
     </row>
-    <row r="44" spans="2:23" ht="30" customHeight="1">
+    <row r="44" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B44" s="5"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -1985,7 +2043,7 @@
       <c r="V44" s="4"/>
       <c r="W44" s="4"/>
     </row>
-    <row r="45" spans="2:23" ht="30" customHeight="1">
+    <row r="45" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B45" s="5"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -2009,7 +2067,7 @@
       <c r="V45" s="4"/>
       <c r="W45" s="4"/>
     </row>
-    <row r="46" spans="2:23" ht="30" customHeight="1">
+    <row r="46" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B46" s="5"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -2033,7 +2091,7 @@
       <c r="V46" s="4"/>
       <c r="W46" s="4"/>
     </row>
-    <row r="47" spans="2:23" ht="30" customHeight="1">
+    <row r="47" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B47" s="5"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -2057,7 +2115,7 @@
       <c r="V47" s="4"/>
       <c r="W47" s="4"/>
     </row>
-    <row r="48" spans="2:23" ht="30" customHeight="1">
+    <row r="48" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B48" s="5"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -2081,7 +2139,7 @@
       <c r="V48" s="4"/>
       <c r="W48" s="4"/>
     </row>
-    <row r="49" spans="2:23" ht="30" customHeight="1">
+    <row r="49" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B49" s="5"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -2105,7 +2163,7 @@
       <c r="V49" s="4"/>
       <c r="W49" s="4"/>
     </row>
-    <row r="50" spans="2:23" ht="30" customHeight="1">
+    <row r="50" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B50" s="5"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -2129,7 +2187,7 @@
       <c r="V50" s="4"/>
       <c r="W50" s="4"/>
     </row>
-    <row r="51" spans="2:23" ht="30" customHeight="1">
+    <row r="51" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B51" s="5"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -2153,7 +2211,7 @@
       <c r="V51" s="4"/>
       <c r="W51" s="4"/>
     </row>
-    <row r="52" spans="2:23" ht="30" customHeight="1">
+    <row r="52" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B52" s="5"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -2177,7 +2235,7 @@
       <c r="V52" s="4"/>
       <c r="W52" s="4"/>
     </row>
-    <row r="53" spans="2:23" ht="30" customHeight="1">
+    <row r="53" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B53" s="5"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -2201,7 +2259,7 @@
       <c r="V53" s="4"/>
       <c r="W53" s="4"/>
     </row>
-    <row r="54" spans="2:23" ht="30" customHeight="1">
+    <row r="54" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B54" s="5"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -2225,7 +2283,7 @@
       <c r="V54" s="4"/>
       <c r="W54" s="4"/>
     </row>
-    <row r="55" spans="2:23" ht="30" customHeight="1">
+    <row r="55" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B55" s="5"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -2249,7 +2307,7 @@
       <c r="V55" s="4"/>
       <c r="W55" s="4"/>
     </row>
-    <row r="56" spans="2:23" ht="30" customHeight="1">
+    <row r="56" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B56" s="5"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -2273,7 +2331,7 @@
       <c r="V56" s="4"/>
       <c r="W56" s="4"/>
     </row>
-    <row r="57" spans="2:23" ht="30" customHeight="1">
+    <row r="57" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B57" s="5"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -2297,7 +2355,7 @@
       <c r="V57" s="4"/>
       <c r="W57" s="4"/>
     </row>
-    <row r="58" spans="2:23" ht="30" customHeight="1">
+    <row r="58" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B58" s="5"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -2321,7 +2379,7 @@
       <c r="V58" s="4"/>
       <c r="W58" s="4"/>
     </row>
-    <row r="59" spans="2:23" ht="30" customHeight="1">
+    <row r="59" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B59" s="5"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -2345,7 +2403,7 @@
       <c r="V59" s="4"/>
       <c r="W59" s="4"/>
     </row>
-    <row r="60" spans="2:23" ht="30" customHeight="1">
+    <row r="60" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B60" s="5"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -2369,7 +2427,7 @@
       <c r="V60" s="4"/>
       <c r="W60" s="4"/>
     </row>
-    <row r="61" spans="2:23" ht="30" customHeight="1">
+    <row r="61" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B61" s="5"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -2393,7 +2451,7 @@
       <c r="V61" s="4"/>
       <c r="W61" s="4"/>
     </row>
-    <row r="62" spans="2:23" ht="30" customHeight="1">
+    <row r="62" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B62" s="5"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -2417,7 +2475,7 @@
       <c r="V62" s="4"/>
       <c r="W62" s="4"/>
     </row>
-    <row r="63" spans="2:23" ht="30" customHeight="1">
+    <row r="63" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B63" s="5"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -2441,7 +2499,7 @@
       <c r="V63" s="4"/>
       <c r="W63" s="4"/>
     </row>
-    <row r="64" spans="2:23" ht="30" customHeight="1">
+    <row r="64" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B64" s="5"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
@@ -2465,7 +2523,7 @@
       <c r="V64" s="4"/>
       <c r="W64" s="4"/>
     </row>
-    <row r="65" spans="2:23" ht="30" customHeight="1">
+    <row r="65" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B65" s="5"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
@@ -2489,7 +2547,7 @@
       <c r="V65" s="4"/>
       <c r="W65" s="4"/>
     </row>
-    <row r="66" spans="2:23" ht="30" customHeight="1">
+    <row r="66" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B66" s="5"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
@@ -2513,7 +2571,7 @@
       <c r="V66" s="4"/>
       <c r="W66" s="4"/>
     </row>
-    <row r="67" spans="2:23" ht="30" customHeight="1">
+    <row r="67" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B67" s="5"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
@@ -2537,7 +2595,7 @@
       <c r="V67" s="4"/>
       <c r="W67" s="4"/>
     </row>
-    <row r="68" spans="2:23" ht="30" customHeight="1">
+    <row r="68" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B68" s="5"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -2561,7 +2619,7 @@
       <c r="V68" s="4"/>
       <c r="W68" s="4"/>
     </row>
-    <row r="69" spans="2:23" ht="30" customHeight="1">
+    <row r="69" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B69" s="5"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
@@ -2585,7 +2643,7 @@
       <c r="V69" s="4"/>
       <c r="W69" s="4"/>
     </row>
-    <row r="70" spans="2:23" ht="30" customHeight="1">
+    <row r="70" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B70" s="5"/>
       <c r="C70" s="6"/>
       <c r="D70" s="6"/>
@@ -2609,7 +2667,7 @@
       <c r="V70" s="7"/>
       <c r="W70" s="4"/>
     </row>
-    <row r="71" spans="2:23" ht="30" customHeight="1">
+    <row r="71" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B71" s="5"/>
       <c r="C71" s="6"/>
       <c r="D71" s="6"/>
@@ -2633,7 +2691,7 @@
       <c r="V71" s="7"/>
       <c r="W71" s="4"/>
     </row>
-    <row r="72" spans="2:23" ht="30" customHeight="1">
+    <row r="72" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B72" s="5"/>
       <c r="C72" s="6"/>
       <c r="D72" s="6"/>
@@ -2657,7 +2715,7 @@
       <c r="V72" s="7"/>
       <c r="W72" s="4"/>
     </row>
-    <row r="73" spans="2:23" ht="30" customHeight="1">
+    <row r="73" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B73" s="5"/>
       <c r="C73" s="6"/>
       <c r="D73" s="6"/>
@@ -2681,7 +2739,7 @@
       <c r="V73" s="7"/>
       <c r="W73" s="4"/>
     </row>
-    <row r="74" spans="2:23" ht="30" customHeight="1">
+    <row r="74" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B74" s="5"/>
       <c r="C74" s="6"/>
       <c r="D74" s="6"/>
@@ -2705,7 +2763,7 @@
       <c r="V74" s="7"/>
       <c r="W74" s="4"/>
     </row>
-    <row r="75" spans="2:23" ht="30" customHeight="1">
+    <row r="75" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B75" s="5"/>
       <c r="C75" s="6"/>
       <c r="D75" s="6"/>
@@ -2729,7 +2787,7 @@
       <c r="V75" s="7"/>
       <c r="W75" s="4"/>
     </row>
-    <row r="76" spans="2:23" ht="30" customHeight="1">
+    <row r="76" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B76" s="5"/>
       <c r="C76" s="6"/>
       <c r="D76" s="6"/>
@@ -2753,7 +2811,7 @@
       <c r="V76" s="7"/>
       <c r="W76" s="4"/>
     </row>
-    <row r="77" spans="2:23" ht="30" customHeight="1">
+    <row r="77" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B77" s="5"/>
       <c r="C77" s="6"/>
       <c r="D77" s="6"/>
@@ -2777,7 +2835,7 @@
       <c r="V77" s="7"/>
       <c r="W77" s="4"/>
     </row>
-    <row r="78" spans="2:23" ht="30" customHeight="1">
+    <row r="78" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B78" s="5"/>
       <c r="C78" s="6"/>
       <c r="D78" s="6"/>
@@ -2801,7 +2859,7 @@
       <c r="V78" s="7"/>
       <c r="W78" s="4"/>
     </row>
-    <row r="79" spans="2:23" ht="30" customHeight="1">
+    <row r="79" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B79" s="5"/>
       <c r="C79" s="6"/>
       <c r="D79" s="6"/>
@@ -2825,7 +2883,7 @@
       <c r="V79" s="7"/>
       <c r="W79" s="4"/>
     </row>
-    <row r="80" spans="2:23" ht="30" customHeight="1">
+    <row r="80" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B80" s="5"/>
       <c r="C80" s="6"/>
       <c r="D80" s="6"/>
@@ -2849,7 +2907,7 @@
       <c r="V80" s="7"/>
       <c r="W80" s="4"/>
     </row>
-    <row r="81" spans="2:23" ht="30" customHeight="1">
+    <row r="81" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B81" s="5"/>
       <c r="C81" s="6"/>
       <c r="D81" s="6"/>
@@ -2873,7 +2931,7 @@
       <c r="V81" s="7"/>
       <c r="W81" s="4"/>
     </row>
-    <row r="82" spans="2:23" ht="30" customHeight="1">
+    <row r="82" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B82" s="5"/>
       <c r="C82" s="6"/>
       <c r="D82" s="6"/>
@@ -2897,7 +2955,7 @@
       <c r="V82" s="7"/>
       <c r="W82" s="4"/>
     </row>
-    <row r="83" spans="2:23" ht="30" customHeight="1">
+    <row r="83" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B83" s="5"/>
       <c r="C83" s="6"/>
       <c r="D83" s="6"/>
@@ -2921,7 +2979,7 @@
       <c r="V83" s="7"/>
       <c r="W83" s="4"/>
     </row>
-    <row r="84" spans="2:23" ht="30" customHeight="1">
+    <row r="84" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B84" s="5"/>
       <c r="C84" s="6"/>
       <c r="D84" s="6"/>
@@ -2945,7 +3003,7 @@
       <c r="V84" s="7"/>
       <c r="W84" s="4"/>
     </row>
-    <row r="85" spans="2:23" ht="30" customHeight="1">
+    <row r="85" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B85" s="5"/>
       <c r="C85" s="6"/>
       <c r="D85" s="6"/>
@@ -2969,7 +3027,7 @@
       <c r="V85" s="7"/>
       <c r="W85" s="4"/>
     </row>
-    <row r="86" spans="2:23" ht="30" customHeight="1">
+    <row r="86" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B86" s="5"/>
       <c r="C86" s="6"/>
       <c r="D86" s="6"/>
@@ -2993,7 +3051,7 @@
       <c r="V86" s="7"/>
       <c r="W86" s="4"/>
     </row>
-    <row r="87" spans="2:23" ht="30" customHeight="1">
+    <row r="87" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B87" s="5"/>
       <c r="C87" s="6"/>
       <c r="D87" s="6"/>
@@ -3017,7 +3075,7 @@
       <c r="V87" s="7"/>
       <c r="W87" s="4"/>
     </row>
-    <row r="88" spans="2:23" ht="30" customHeight="1">
+    <row r="88" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B88" s="5"/>
       <c r="C88" s="6"/>
       <c r="D88" s="6"/>
@@ -3041,7 +3099,7 @@
       <c r="V88" s="7"/>
       <c r="W88" s="4"/>
     </row>
-    <row r="89" spans="2:23" ht="30" customHeight="1">
+    <row r="89" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B89" s="5"/>
       <c r="C89" s="6"/>
       <c r="D89" s="6"/>
@@ -3065,7 +3123,7 @@
       <c r="V89" s="7"/>
       <c r="W89" s="4"/>
     </row>
-    <row r="90" spans="2:23" ht="30" customHeight="1">
+    <row r="90" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B90" s="5"/>
       <c r="C90" s="6"/>
       <c r="D90" s="6"/>
@@ -3089,7 +3147,7 @@
       <c r="V90" s="7"/>
       <c r="W90" s="4"/>
     </row>
-    <row r="91" spans="2:23" ht="30" customHeight="1">
+    <row r="91" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B91" s="5"/>
       <c r="C91" s="6"/>
       <c r="D91" s="6"/>
@@ -3113,7 +3171,7 @@
       <c r="V91" s="7"/>
       <c r="W91" s="4"/>
     </row>
-    <row r="92" spans="2:23" ht="30" customHeight="1">
+    <row r="92" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B92" s="5"/>
       <c r="C92" s="6"/>
       <c r="D92" s="6"/>
@@ -3137,7 +3195,7 @@
       <c r="V92" s="7"/>
       <c r="W92" s="4"/>
     </row>
-    <row r="93" spans="2:23" ht="30" customHeight="1">
+    <row r="93" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B93" s="5"/>
       <c r="C93" s="6"/>
       <c r="D93" s="6"/>
@@ -3161,7 +3219,7 @@
       <c r="V93" s="7"/>
       <c r="W93" s="4"/>
     </row>
-    <row r="94" spans="2:23" ht="30" customHeight="1">
+    <row r="94" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B94" s="5"/>
       <c r="C94" s="6"/>
       <c r="D94" s="6"/>
@@ -3185,7 +3243,7 @@
       <c r="V94" s="7"/>
       <c r="W94" s="4"/>
     </row>
-    <row r="95" spans="2:23" ht="30" customHeight="1">
+    <row r="95" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B95" s="5"/>
       <c r="C95" s="6"/>
       <c r="D95" s="6"/>
@@ -3209,7 +3267,7 @@
       <c r="V95" s="7"/>
       <c r="W95" s="4"/>
     </row>
-    <row r="96" spans="2:23" ht="30" customHeight="1">
+    <row r="96" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B96" s="5"/>
       <c r="C96" s="6"/>
       <c r="D96" s="6"/>
@@ -3233,7 +3291,7 @@
       <c r="V96" s="7"/>
       <c r="W96" s="4"/>
     </row>
-    <row r="97" spans="2:23" ht="30" customHeight="1">
+    <row r="97" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B97" s="5"/>
       <c r="C97" s="6"/>
       <c r="D97" s="6"/>
@@ -3257,7 +3315,7 @@
       <c r="V97" s="7"/>
       <c r="W97" s="4"/>
     </row>
-    <row r="98" spans="2:23" ht="30" customHeight="1">
+    <row r="98" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B98" s="5"/>
       <c r="C98" s="6"/>
       <c r="D98" s="6"/>
@@ -3281,7 +3339,7 @@
       <c r="V98" s="7"/>
       <c r="W98" s="4"/>
     </row>
-    <row r="99" spans="2:23" ht="30" customHeight="1">
+    <row r="99" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B99" s="5"/>
       <c r="C99" s="6"/>
       <c r="D99" s="6"/>
@@ -3305,7 +3363,7 @@
       <c r="V99" s="7"/>
       <c r="W99" s="4"/>
     </row>
-    <row r="100" spans="2:23" ht="30" customHeight="1">
+    <row r="100" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B100" s="5"/>
       <c r="C100" s="6"/>
       <c r="D100" s="6"/>
@@ -3329,7 +3387,7 @@
       <c r="V100" s="7"/>
       <c r="W100" s="4"/>
     </row>
-    <row r="101" spans="2:23" ht="30" customHeight="1">
+    <row r="101" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B101" s="5"/>
       <c r="C101" s="6"/>
       <c r="D101" s="6"/>
@@ -3353,7 +3411,7 @@
       <c r="V101" s="7"/>
       <c r="W101" s="4"/>
     </row>
-    <row r="102" spans="2:23" ht="30" customHeight="1">
+    <row r="102" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B102" s="5"/>
       <c r="C102" s="6"/>
       <c r="D102" s="6"/>
@@ -3377,7 +3435,7 @@
       <c r="V102" s="7"/>
       <c r="W102" s="4"/>
     </row>
-    <row r="103" spans="2:23" ht="30" customHeight="1">
+    <row r="103" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B103" s="5"/>
       <c r="C103" s="6"/>
       <c r="D103" s="6"/>
@@ -3401,7 +3459,7 @@
       <c r="V103" s="7"/>
       <c r="W103" s="4"/>
     </row>
-    <row r="104" spans="2:23" ht="30" customHeight="1">
+    <row r="104" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B104" s="5"/>
       <c r="C104" s="6"/>
       <c r="D104" s="6"/>
@@ -3425,7 +3483,7 @@
       <c r="V104" s="7"/>
       <c r="W104" s="4"/>
     </row>
-    <row r="105" spans="2:23" ht="30" customHeight="1">
+    <row r="105" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B105" s="5"/>
       <c r="C105" s="6"/>
       <c r="D105" s="6"/>
@@ -3449,7 +3507,7 @@
       <c r="V105" s="7"/>
       <c r="W105" s="4"/>
     </row>
-    <row r="106" spans="2:23" ht="30" customHeight="1">
+    <row r="106" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B106" s="5"/>
       <c r="C106" s="6"/>
       <c r="D106" s="6"/>
@@ -3473,7 +3531,7 @@
       <c r="V106" s="7"/>
       <c r="W106" s="4"/>
     </row>
-    <row r="107" spans="2:23" ht="30" customHeight="1">
+    <row r="107" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B107" s="5"/>
       <c r="C107" s="6"/>
       <c r="D107" s="6"/>
@@ -3497,7 +3555,7 @@
       <c r="V107" s="7"/>
       <c r="W107" s="4"/>
     </row>
-    <row r="108" spans="2:23" ht="30" customHeight="1">
+    <row r="108" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B108" s="5"/>
       <c r="C108" s="6"/>
       <c r="D108" s="6"/>
@@ -3521,7 +3579,7 @@
       <c r="V108" s="7"/>
       <c r="W108" s="4"/>
     </row>
-    <row r="109" spans="2:23" ht="30" customHeight="1">
+    <row r="109" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B109" s="5"/>
       <c r="C109" s="6"/>
       <c r="D109" s="6"/>
@@ -3545,7 +3603,7 @@
       <c r="V109" s="7"/>
       <c r="W109" s="4"/>
     </row>
-    <row r="110" spans="2:23" ht="30" customHeight="1">
+    <row r="110" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B110" s="5"/>
       <c r="C110" s="6"/>
       <c r="D110" s="6"/>
@@ -3569,7 +3627,7 @@
       <c r="V110" s="7"/>
       <c r="W110" s="4"/>
     </row>
-    <row r="111" spans="2:23" ht="30" customHeight="1">
+    <row r="111" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B111" s="5"/>
       <c r="C111" s="6"/>
       <c r="D111" s="6"/>
@@ -3593,7 +3651,7 @@
       <c r="V111" s="7"/>
       <c r="W111" s="4"/>
     </row>
-    <row r="112" spans="2:23" ht="30" customHeight="1">
+    <row r="112" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B112" s="5"/>
       <c r="C112" s="6"/>
       <c r="D112" s="6"/>
@@ -3617,7 +3675,7 @@
       <c r="V112" s="7"/>
       <c r="W112" s="4"/>
     </row>
-    <row r="113" spans="2:23" ht="30" customHeight="1">
+    <row r="113" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B113" s="5"/>
       <c r="C113" s="6"/>
       <c r="D113" s="6"/>
@@ -3641,7 +3699,7 @@
       <c r="V113" s="7"/>
       <c r="W113" s="4"/>
     </row>
-    <row r="114" spans="2:23" ht="30" customHeight="1">
+    <row r="114" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B114" s="5"/>
       <c r="C114" s="6"/>
       <c r="D114" s="6"/>
@@ -3665,7 +3723,7 @@
       <c r="V114" s="7"/>
       <c r="W114" s="4"/>
     </row>
-    <row r="115" spans="2:23" ht="30" customHeight="1">
+    <row r="115" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B115" s="5"/>
       <c r="C115" s="6"/>
       <c r="D115" s="6"/>
@@ -3689,7 +3747,7 @@
       <c r="V115" s="7"/>
       <c r="W115" s="4"/>
     </row>
-    <row r="116" spans="2:23" ht="30" customHeight="1">
+    <row r="116" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B116" s="5"/>
       <c r="C116" s="6"/>
       <c r="D116" s="6"/>
@@ -3713,7 +3771,7 @@
       <c r="V116" s="7"/>
       <c r="W116" s="4"/>
     </row>
-    <row r="117" spans="2:23" ht="30" customHeight="1">
+    <row r="117" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B117" s="5"/>
       <c r="C117" s="6"/>
       <c r="D117" s="6"/>
@@ -3737,7 +3795,7 @@
       <c r="V117" s="7"/>
       <c r="W117" s="4"/>
     </row>
-    <row r="118" spans="2:23" ht="30" customHeight="1">
+    <row r="118" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B118" s="5"/>
       <c r="C118" s="6"/>
       <c r="D118" s="6"/>
@@ -3761,7 +3819,7 @@
       <c r="V118" s="7"/>
       <c r="W118" s="4"/>
     </row>
-    <row r="119" spans="2:23" ht="30" customHeight="1">
+    <row r="119" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B119" s="5"/>
       <c r="C119" s="6"/>
       <c r="D119" s="6"/>
@@ -3785,7 +3843,7 @@
       <c r="V119" s="7"/>
       <c r="W119" s="4"/>
     </row>
-    <row r="120" spans="2:23" ht="30" customHeight="1">
+    <row r="120" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B120" s="5"/>
       <c r="C120" s="6"/>
       <c r="D120" s="6"/>
@@ -3809,7 +3867,7 @@
       <c r="V120" s="7"/>
       <c r="W120" s="4"/>
     </row>
-    <row r="121" spans="2:23" ht="30" customHeight="1">
+    <row r="121" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B121" s="5"/>
       <c r="C121" s="6"/>
       <c r="D121" s="6"/>
@@ -3833,7 +3891,7 @@
       <c r="V121" s="7"/>
       <c r="W121" s="4"/>
     </row>
-    <row r="122" spans="2:23" ht="30" customHeight="1">
+    <row r="122" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B122" s="5"/>
       <c r="C122" s="6"/>
       <c r="D122" s="6"/>
@@ -3857,7 +3915,7 @@
       <c r="V122" s="7"/>
       <c r="W122" s="4"/>
     </row>
-    <row r="123" spans="2:23" ht="30" customHeight="1">
+    <row r="123" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B123" s="5"/>
       <c r="C123" s="6"/>
       <c r="D123" s="6"/>
@@ -3881,7 +3939,7 @@
       <c r="V123" s="7"/>
       <c r="W123" s="4"/>
     </row>
-    <row r="124" spans="2:23" ht="30" customHeight="1">
+    <row r="124" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B124" s="5"/>
       <c r="C124" s="6"/>
       <c r="D124" s="6"/>
@@ -3905,7 +3963,7 @@
       <c r="V124" s="7"/>
       <c r="W124" s="4"/>
     </row>
-    <row r="125" spans="2:23" ht="30" customHeight="1">
+    <row r="125" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B125" s="5"/>
       <c r="C125" s="6"/>
       <c r="D125" s="6"/>
@@ -3929,7 +3987,7 @@
       <c r="V125" s="7"/>
       <c r="W125" s="4"/>
     </row>
-    <row r="126" spans="2:23" ht="30" customHeight="1">
+    <row r="126" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B126" s="5"/>
       <c r="C126" s="6"/>
       <c r="D126" s="6"/>
@@ -3953,7 +4011,7 @@
       <c r="V126" s="7"/>
       <c r="W126" s="4"/>
     </row>
-    <row r="127" spans="2:23" ht="30" customHeight="1">
+    <row r="127" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B127" s="5"/>
       <c r="C127" s="6"/>
       <c r="D127" s="6"/>
@@ -3977,7 +4035,7 @@
       <c r="V127" s="7"/>
       <c r="W127" s="4"/>
     </row>
-    <row r="128" spans="2:23" ht="30" customHeight="1">
+    <row r="128" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B128" s="5"/>
       <c r="C128" s="6"/>
       <c r="D128" s="6"/>
@@ -4001,7 +4059,7 @@
       <c r="V128" s="7"/>
       <c r="W128" s="4"/>
     </row>
-    <row r="129" spans="2:23" ht="30" customHeight="1">
+    <row r="129" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B129" s="5"/>
       <c r="C129" s="6"/>
       <c r="D129" s="6"/>
@@ -4025,7 +4083,7 @@
       <c r="V129" s="7"/>
       <c r="W129" s="4"/>
     </row>
-    <row r="130" spans="2:23" ht="30" customHeight="1">
+    <row r="130" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B130" s="5"/>
       <c r="C130" s="6"/>
       <c r="D130" s="6"/>
@@ -4049,7 +4107,7 @@
       <c r="V130" s="7"/>
       <c r="W130" s="4"/>
     </row>
-    <row r="131" spans="2:23" ht="30" customHeight="1">
+    <row r="131" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B131" s="5"/>
       <c r="C131" s="6"/>
       <c r="D131" s="6"/>
@@ -4073,7 +4131,7 @@
       <c r="V131" s="7"/>
       <c r="W131" s="4"/>
     </row>
-    <row r="132" spans="2:23" ht="30" customHeight="1">
+    <row r="132" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B132" s="5"/>
       <c r="C132" s="6"/>
       <c r="D132" s="6"/>
@@ -4097,7 +4155,7 @@
       <c r="V132" s="7"/>
       <c r="W132" s="4"/>
     </row>
-    <row r="133" spans="2:23" ht="30" customHeight="1">
+    <row r="133" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B133" s="5"/>
       <c r="C133" s="6"/>
       <c r="D133" s="6"/>
@@ -4121,7 +4179,7 @@
       <c r="V133" s="7"/>
       <c r="W133" s="4"/>
     </row>
-    <row r="134" spans="2:23" ht="30" customHeight="1">
+    <row r="134" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B134" s="5"/>
       <c r="C134" s="6"/>
       <c r="D134" s="6"/>
@@ -4145,7 +4203,7 @@
       <c r="V134" s="7"/>
       <c r="W134" s="4"/>
     </row>
-    <row r="135" spans="2:23" ht="30" customHeight="1">
+    <row r="135" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B135" s="5"/>
       <c r="C135" s="6"/>
       <c r="D135" s="6"/>
@@ -4169,7 +4227,7 @@
       <c r="V135" s="7"/>
       <c r="W135" s="4"/>
     </row>
-    <row r="136" spans="2:23" ht="30" customHeight="1">
+    <row r="136" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B136" s="5"/>
       <c r="C136" s="6"/>
       <c r="D136" s="6"/>
@@ -4193,7 +4251,7 @@
       <c r="V136" s="7"/>
       <c r="W136" s="4"/>
     </row>
-    <row r="137" spans="2:23" ht="30" customHeight="1">
+    <row r="137" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B137" s="5"/>
       <c r="C137" s="6"/>
       <c r="D137" s="6"/>
@@ -4217,7 +4275,7 @@
       <c r="V137" s="7"/>
       <c r="W137" s="4"/>
     </row>
-    <row r="138" spans="2:23" ht="30" customHeight="1">
+    <row r="138" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B138" s="5"/>
       <c r="C138" s="6"/>
       <c r="D138" s="6"/>
@@ -4241,7 +4299,7 @@
       <c r="V138" s="7"/>
       <c r="W138" s="4"/>
     </row>
-    <row r="139" spans="2:23" ht="30" customHeight="1">
+    <row r="139" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B139" s="5"/>
       <c r="C139" s="6"/>
       <c r="D139" s="6"/>
@@ -4265,7 +4323,7 @@
       <c r="V139" s="7"/>
       <c r="W139" s="4"/>
     </row>
-    <row r="140" spans="2:23" ht="30" customHeight="1">
+    <row r="140" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B140" s="5"/>
       <c r="C140" s="6"/>
       <c r="D140" s="6"/>
@@ -4289,7 +4347,7 @@
       <c r="V140" s="7"/>
       <c r="W140" s="4"/>
     </row>
-    <row r="141" spans="2:23" ht="30" customHeight="1">
+    <row r="141" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B141" s="5"/>
       <c r="C141" s="6"/>
       <c r="D141" s="6"/>
@@ -4313,7 +4371,7 @@
       <c r="V141" s="7"/>
       <c r="W141" s="4"/>
     </row>
-    <row r="142" spans="2:23" ht="30" customHeight="1">
+    <row r="142" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B142" s="5"/>
       <c r="C142" s="6"/>
       <c r="D142" s="6"/>
@@ -4337,7 +4395,7 @@
       <c r="V142" s="7"/>
       <c r="W142" s="4"/>
     </row>
-    <row r="143" spans="2:23" ht="30" customHeight="1">
+    <row r="143" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B143" s="5"/>
       <c r="C143" s="6"/>
       <c r="D143" s="6"/>
@@ -4361,7 +4419,7 @@
       <c r="V143" s="7"/>
       <c r="W143" s="4"/>
     </row>
-    <row r="144" spans="2:23" ht="30" customHeight="1">
+    <row r="144" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B144" s="5"/>
       <c r="C144" s="6"/>
       <c r="D144" s="6"/>
@@ -4385,95 +4443,110 @@
       <c r="V144" s="7"/>
       <c r="W144" s="4"/>
     </row>
-    <row r="145" spans="2:23" ht="30" customHeight="1">
+    <row r="145" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B145" s="8"/>
       <c r="W145" s="9"/>
     </row>
-    <row r="146" spans="2:23" ht="30" customHeight="1">
+    <row r="146" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B146" s="8"/>
       <c r="W146" s="9"/>
     </row>
-    <row r="147" spans="2:23" ht="30" customHeight="1">
+    <row r="147" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B147" s="8"/>
       <c r="W147" s="9"/>
     </row>
-    <row r="148" spans="2:23" ht="30" customHeight="1">
+    <row r="148" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B148" s="8"/>
       <c r="W148" s="9"/>
     </row>
-    <row r="149" spans="2:23" ht="30" customHeight="1">
+    <row r="149" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B149" s="8"/>
       <c r="W149" s="9"/>
     </row>
-    <row r="150" spans="2:23" ht="30" customHeight="1">
+    <row r="150" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B150" s="8"/>
       <c r="W150" s="9"/>
     </row>
-    <row r="151" spans="2:23" ht="30" customHeight="1">
+    <row r="151" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B151" s="8"/>
       <c r="W151" s="9"/>
     </row>
-    <row r="152" spans="2:23" ht="30" customHeight="1">
+    <row r="152" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B152" s="8"/>
       <c r="W152" s="9"/>
     </row>
-    <row r="153" spans="2:23" ht="30" customHeight="1">
+    <row r="153" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B153" s="8"/>
       <c r="W153" s="9"/>
     </row>
-    <row r="154" spans="2:23" ht="30" customHeight="1">
+    <row r="154" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B154" s="8"/>
       <c r="W154" s="9"/>
     </row>
-    <row r="155" spans="2:23" ht="30" customHeight="1">
+    <row r="155" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B155" s="8"/>
       <c r="W155" s="9"/>
     </row>
-    <row r="156" spans="2:23" ht="30" customHeight="1">
+    <row r="156" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B156" s="8"/>
       <c r="W156" s="9"/>
     </row>
-    <row r="157" spans="2:23" ht="30" customHeight="1">
+    <row r="157" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B157" s="8"/>
       <c r="W157" s="9"/>
     </row>
-    <row r="158" spans="2:23" ht="30" customHeight="1">
+    <row r="158" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B158" s="8"/>
       <c r="W158" s="9"/>
     </row>
-    <row r="159" spans="2:23" ht="30" customHeight="1">
+    <row r="159" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B159" s="8"/>
       <c r="W159" s="9"/>
     </row>
-    <row r="160" spans="2:23" ht="30" customHeight="1">
+    <row r="160" spans="2:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B160" s="8"/>
     </row>
-    <row r="161" spans="2:2" ht="30" customHeight="1">
+    <row r="161" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B161" s="8"/>
     </row>
-    <row r="162" spans="2:2" ht="30" customHeight="1">
+    <row r="162" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B162" s="8"/>
     </row>
-    <row r="163" spans="2:2" ht="30" customHeight="1">
+    <row r="163" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B163" s="8"/>
     </row>
-    <row r="164" spans="2:2" ht="30" customHeight="1">
+    <row r="164" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B164" s="8"/>
     </row>
-    <row r="165" spans="2:2" ht="30" customHeight="1">
+    <row r="165" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B165" s="8"/>
     </row>
-    <row r="166" spans="2:2" ht="30" customHeight="1">
+    <row r="166" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B166" s="8"/>
     </row>
-    <row r="167" spans="2:2" ht="30" customHeight="1">
+    <row r="167" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B167" s="8"/>
     </row>
-    <row r="168" spans="2:2" ht="30" customHeight="1">
+    <row r="168" spans="2:2" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B168" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="V2:V3"/>
     <mergeCell ref="W2:W3"/>
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="N2:N3"/>
@@ -4482,21 +4555,6 @@
     <mergeCell ref="R2:R3"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="P2:P3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>